<commit_message>
Merge Version from Shivank for 17Jan26
</commit_message>
<xml_diff>
--- a/tests/ManualTests.xlsx
+++ b/tests/ManualTests.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GoSewa\GoSEWA\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F0818E-4676-40D8-B16F-6F181375B525}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DCA585-87AA-48CA-9D49-D39FE37172D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{44483A70-9FE6-4AE3-BD92-0A8604EB7277}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login Page" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Login Page'!$A$1:$G$10</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="36">
   <si>
     <t>Test tracker</t>
   </si>
@@ -33,9 +36,6 @@
     <t>Loginn Page</t>
   </si>
   <si>
-    <t>Signup</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
@@ -121,6 +121,21 @@
   </si>
   <si>
     <t>1.3.1</t>
+  </si>
+  <si>
+    <t>User should be able to login or create user</t>
+  </si>
+  <si>
+    <t>Signup Page</t>
+  </si>
+  <si>
+    <t>User correct data</t>
+  </si>
+  <si>
+    <t>Current Status</t>
+  </si>
+  <si>
+    <t>Fixed</t>
   </si>
 </sst>
 </file>
@@ -492,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60F0DE0-6F0F-4992-924D-11CFFEC40623}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,171 +525,193 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>1.1000000000000001</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>25</v>
+      <c r="H10" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G10" xr:uid="{9414561E-4B2C-40E1-9E11-6E1BAF808535}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>